<commit_message>
mods for chapter 4 of dissertation
</commit_message>
<xml_diff>
--- a/profile data/Hypothesis Tests.xlsx
+++ b/profile data/Hypothesis Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="18780" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="31420" windowHeight="18780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,40 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>Var(X)</t>
-  </si>
-  <si>
-    <t>Std(X)</t>
-  </si>
-  <si>
-    <t>Obs. X</t>
-  </si>
-  <si>
-    <t>E(X)</t>
-  </si>
-  <si>
-    <t>Standardized X</t>
-  </si>
-  <si>
-    <t>H0:  Agent answer rate = 0.454</t>
-  </si>
-  <si>
-    <t>H1: Agent answer rate &gt; 0.454</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Question Count: </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
   <si>
     <t>E(Question Score):</t>
   </si>
@@ -78,17 +45,90 @@
     <t>Z-score for p-value of 1%</t>
   </si>
   <si>
-    <t>Conclusion:  Reject H0 in favor of H1 at a p-value &lt; 0.01</t>
+    <t>Concept Match V2 vs. Max Frequency</t>
+  </si>
+  <si>
+    <t>Concept Match V3 vs. Concept Match V2</t>
+  </si>
+  <si>
+    <t>Conclusion:  Accept H0.</t>
+  </si>
+  <si>
+    <t>Concept Match Not vs. Random</t>
+  </si>
+  <si>
+    <t>Z-score for p-value of 2%</t>
+  </si>
+  <si>
+    <t>Conclusion:  Reject H0 in favor of H1 at the 98% confidence level</t>
+  </si>
+  <si>
+    <t>Conclusion:  Reject H0 in favor of H1 at the 99% confidence level</t>
+  </si>
+  <si>
+    <t>H0:  Agent accuracy = 25%</t>
+  </si>
+  <si>
+    <t>H1: Agent accuracy &gt; 25%</t>
+  </si>
+  <si>
+    <t>Number of Exam Questions:</t>
+  </si>
+  <si>
+    <t>H0:  Agent accuracy = 60.2%</t>
+  </si>
+  <si>
+    <t>H1: Agent accuracy &gt; 60.2%</t>
+  </si>
+  <si>
+    <t>H0:  Agent accuracy = 45.4%</t>
+  </si>
+  <si>
+    <t>H1: Agent accuracy &gt; 45.4%</t>
+  </si>
+  <si>
+    <t>Conclusion:  Reject H0 in favor of H1 at the 99% confidence level (p-value &lt; 0.01)</t>
+  </si>
+  <si>
+    <t>Concept Match NOTA vs. Max Freq</t>
+  </si>
+  <si>
+    <t>H0:  Agent accuracy = 55%</t>
+  </si>
+  <si>
+    <t>H1: Agent accuracy &gt; 55%</t>
+  </si>
+  <si>
+    <t>(0.01 &lt; p-value &lt; 0.02)</t>
+  </si>
+  <si>
+    <t>CFE Agent Version 2 vs. CFE Agent Version 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,13 +151,85 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="37">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,172 +559,520 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K17"/>
+  <dimension ref="B2:D99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="10" max="10" width="21.1640625" customWidth="1"/>
+    <col min="14" max="14" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:4">
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="D7">
         <v>0.45400000000000001</v>
       </c>
     </row>
-    <row r="3" spans="2:11">
-      <c r="B3" t="s">
+    <row r="8" spans="2:4">
+      <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
-        <f>1-C2</f>
-        <v>0.54600000000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11">
-      <c r="B4" t="s">
+      <c r="D8">
+        <f>D7*(1-D7)</f>
+        <v>0.24788400000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="D10">
+        <f>D9*D7</f>
+        <v>88.984000000000009</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <f>D9*D8</f>
+        <v>48.585264000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <f>SQRT(D11)</f>
+        <v>6.9703130489239866</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <f>(D13-D10)/D12</f>
+        <v>4.1627972511907796</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>2.3250000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <f>D27*(1-D27)</f>
+        <v>0.239596</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29">
         <v>196</v>
       </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11">
-      <c r="B5" t="s">
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <f>D29*D27</f>
+        <v>117.99199999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <f>D29*D28</f>
+        <v>46.960816000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <f>SQRT(D31)</f>
+        <v>6.8527962176034389</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
-        <f>C4*C2</f>
-        <v>88.984000000000009</v>
-      </c>
-      <c r="I5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11">
-      <c r="B6" t="s">
+      <c r="D34">
+        <f>(D33-D30)/D32</f>
+        <v>0.43894490722970425</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <v>2.3250000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="B47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <f>D47*(1-D47)</f>
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <f>D49*D47</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
-        <f>C4*C3*C2</f>
-        <v>48.585264000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" t="s">
+      <c r="D51">
+        <f>D49*D48</f>
+        <v>5.0625</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
-        <f>SQRT(C6)</f>
-        <v>6.9703130489239866</v>
-      </c>
-      <c r="I7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" t="s">
+      <c r="D52">
+        <f>SQRT(D51)</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
-        <v>118</v>
-      </c>
-      <c r="I8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8">
-        <v>0.45400000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="B9" t="s">
+      <c r="D53">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <f>(D53-D50)/D52</f>
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55" t="s">
         <v>7</v>
       </c>
-      <c r="C9">
-        <f>(C8-C5)/C7</f>
-        <v>4.1627972511907796</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="D55">
+        <v>2.3250000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="B62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4">
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="B65" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="B67" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="B68" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <f>D67*(1-D67)</f>
+        <v>0.2475</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="B69" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="B70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <f>D69*D67</f>
+        <v>92.95</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4">
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <f>D69*D68</f>
+        <v>41.827500000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4">
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <f>SQRT(D71)</f>
+        <v>6.4674183411930297</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4">
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4">
+      <c r="B74" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74">
+        <f>(D73-D70)/D72</f>
+        <v>2.1724278929833734</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4">
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75">
+        <v>2.3250000000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4">
+      <c r="B76" t="s">
         <v>12</v>
       </c>
-      <c r="K9">
-        <f>K8*(1-K8)</f>
-        <v>0.24788400000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="I10" t="s">
+      <c r="D76">
+        <v>2.0550000000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4">
+      <c r="B78" t="s">
         <v>13</v>
       </c>
-      <c r="K10">
-        <f>0.454</f>
-        <v>0.45400000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11">
-      <c r="I11" t="s">
+    </row>
+    <row r="79" spans="2:4">
+      <c r="B79" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4">
+      <c r="B84" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4">
+      <c r="B86" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4">
+      <c r="B87" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4">
+      <c r="B89" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0.47699999999999998</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4">
+      <c r="B90" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <f>D89*(1-D89)</f>
+        <v>0.249471</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4">
+      <c r="B91" t="s">
+        <v>17</v>
+      </c>
+      <c r="D91">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4">
+      <c r="B92" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92">
+        <f>D91*D89</f>
+        <v>414.036</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4">
+      <c r="B93" t="s">
+        <v>3</v>
+      </c>
+      <c r="D93">
+        <f>D91*D90</f>
+        <v>216.540828</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4">
+      <c r="B94" t="s">
+        <v>4</v>
+      </c>
+      <c r="D94">
+        <f>SQRT(D93)</f>
+        <v>14.715326296076482</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4">
+      <c r="B95" t="s">
+        <v>5</v>
+      </c>
+      <c r="D95">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4">
+      <c r="B96" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96">
+        <f>(D95-D92)/D94</f>
+        <v>4.8904114358094537</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4">
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97">
+        <v>2.3250000000000002</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4">
+      <c r="B99" t="s">
         <v>14</v>
-      </c>
-      <c r="K11">
-        <f>K9/K7</f>
-        <v>1.2647142857142859E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11">
-      <c r="I12" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12">
-        <f>SQRT(K11)</f>
-        <v>3.5562821678183608E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11">
-      <c r="I13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13">
-        <f>0.602</f>
-        <v>0.60199999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11">
-      <c r="I14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14">
-        <f>(K13-K10)/K12</f>
-        <v>4.1616495265557667</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11">
-      <c r="I15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15">
-        <v>2.3250000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="9:9">
-      <c r="I17" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
modified questions such that they map to the proper section of the manual
</commit_message>
<xml_diff>
--- a/profile data/Hypothesis Tests.xlsx
+++ b/profile data/Hypothesis Tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
   <si>
     <t>E(Question Score):</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>CFE Agent Version 2 vs. CFE Agent Version 1</t>
+  </si>
+  <si>
+    <t>Multiple Choice Questions</t>
   </si>
 </sst>
 </file>
@@ -151,8 +154,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -193,7 +198,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -212,6 +217,7 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -230,6 +236,7 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D99"/>
+  <dimension ref="B2:D100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="H93" sqref="H93"/>
+      <selection activeCell="F112" sqref="F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -978,95 +985,100 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="2:4">
-      <c r="B86" t="s">
-        <v>24</v>
+    <row r="85" spans="2:4">
+      <c r="B85" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="87" spans="2:4">
       <c r="B87" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4">
+      <c r="B88" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4">
-      <c r="B89" t="s">
-        <v>0</v>
-      </c>
-      <c r="D89">
-        <v>0.47699999999999998</v>
       </c>
     </row>
     <row r="90" spans="2:4">
       <c r="B90" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D90">
-        <f>D89*(1-D89)</f>
-        <v>0.249471</v>
+        <v>0.47699999999999998</v>
       </c>
     </row>
     <row r="91" spans="2:4">
       <c r="B91" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D91">
-        <v>868</v>
+        <f>D90*(1-D90)</f>
+        <v>0.249471</v>
       </c>
     </row>
     <row r="92" spans="2:4">
       <c r="B92" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D92">
-        <f>D91*D89</f>
-        <v>414.036</v>
+        <v>868</v>
       </c>
     </row>
     <row r="93" spans="2:4">
       <c r="B93" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D93">
-        <f>D91*D90</f>
-        <v>216.540828</v>
+        <f>D92*D90</f>
+        <v>414.036</v>
       </c>
     </row>
     <row r="94" spans="2:4">
       <c r="B94" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D94">
-        <f>SQRT(D93)</f>
-        <v>14.715326296076482</v>
+        <f>D92*D91</f>
+        <v>216.540828</v>
       </c>
     </row>
     <row r="95" spans="2:4">
       <c r="B95" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D95">
-        <v>486</v>
+        <f>SQRT(D94)</f>
+        <v>14.715326296076482</v>
       </c>
     </row>
     <row r="96" spans="2:4">
       <c r="B96" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D96">
-        <f>(D95-D92)/D94</f>
-        <v>4.8904114358094537</v>
+        <v>486</v>
       </c>
     </row>
     <row r="97" spans="2:4">
       <c r="B97" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97">
+        <f>(D96-D93)/D95</f>
+        <v>4.8904114358094537</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4">
+      <c r="B98" t="s">
         <v>7</v>
       </c>
-      <c r="D97">
+      <c r="D98">
         <v>2.3250000000000002</v>
       </c>
     </row>
-    <row r="99" spans="2:4">
-      <c r="B99" t="s">
+    <row r="100" spans="2:4">
+      <c r="B100" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
moved covert examinations questions to sources of information category
</commit_message>
<xml_diff>
--- a/profile data/Hypothesis Tests.xlsx
+++ b/profile data/Hypothesis Tests.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="31420" windowHeight="18780" tabRatio="500"/>
@@ -566,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D100"/>
+  <dimension ref="B2:H100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="F112" sqref="F112"/>
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -880,12 +880,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="2:4">
+    <row r="65" spans="2:8">
       <c r="B65" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="2:4">
+    <row r="67" spans="2:8">
       <c r="B67" t="s">
         <v>0</v>
       </c>
@@ -893,7 +893,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="68" spans="2:4">
+    <row r="68" spans="2:8">
       <c r="B68" t="s">
         <v>1</v>
       </c>
@@ -902,7 +902,7 @@
         <v>0.2475</v>
       </c>
     </row>
-    <row r="69" spans="2:4">
+    <row r="69" spans="2:8">
       <c r="B69" t="s">
         <v>17</v>
       </c>
@@ -910,7 +910,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="70" spans="2:4">
+    <row r="70" spans="2:8">
       <c r="B70" t="s">
         <v>2</v>
       </c>
@@ -919,7 +919,7 @@
         <v>92.95</v>
       </c>
     </row>
-    <row r="71" spans="2:4">
+    <row r="71" spans="2:8">
       <c r="B71" t="s">
         <v>3</v>
       </c>
@@ -928,7 +928,7 @@
         <v>41.827500000000001</v>
       </c>
     </row>
-    <row r="72" spans="2:4">
+    <row r="72" spans="2:8">
       <c r="B72" t="s">
         <v>4</v>
       </c>
@@ -937,15 +937,19 @@
         <v>6.4674183411930297</v>
       </c>
     </row>
-    <row r="73" spans="2:4">
+    <row r="73" spans="2:8">
       <c r="B73" t="s">
         <v>5</v>
       </c>
       <c r="D73">
         <v>107</v>
       </c>
-    </row>
-    <row r="74" spans="2:4">
+      <c r="H73">
+        <f>9*1663</f>
+        <v>14967</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8">
       <c r="B74" t="s">
         <v>6</v>
       </c>
@@ -953,16 +957,23 @@
         <f>(D73-D70)/D72</f>
         <v>2.1724278929833734</v>
       </c>
-    </row>
-    <row r="75" spans="2:4">
+      <c r="H74">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8">
       <c r="B75" t="s">
         <v>7</v>
       </c>
       <c r="D75">
         <v>2.3250000000000002</v>
       </c>
-    </row>
-    <row r="76" spans="2:4">
+      <c r="H75">
+        <f>H73/H74</f>
+        <v>2494.5</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8">
       <c r="B76" t="s">
         <v>12</v>
       </c>
@@ -970,12 +981,12 @@
         <v>2.0550000000000002</v>
       </c>
     </row>
-    <row r="78" spans="2:4">
+    <row r="78" spans="2:8">
       <c r="B78" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="2:4">
+    <row r="79" spans="2:8">
       <c r="B79" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
updated test results for modified/new features from versions 3.0.0-3.0.2
</commit_message>
<xml_diff>
--- a/profile data/Hypothesis Tests.xlsx
+++ b/profile data/Hypothesis Tests.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="31420" windowHeight="18780" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>E(Question Score):</t>
   </si>
@@ -75,30 +75,12 @@
     <t>Number of Exam Questions:</t>
   </si>
   <si>
-    <t>H0:  Agent accuracy = 60.2%</t>
-  </si>
-  <si>
-    <t>H1: Agent accuracy &gt; 60.2%</t>
-  </si>
-  <si>
-    <t>H0:  Agent accuracy = 45.4%</t>
-  </si>
-  <si>
-    <t>H1: Agent accuracy &gt; 45.4%</t>
-  </si>
-  <si>
     <t>Conclusion:  Reject H0 in favor of H1 at the 99% confidence level (p-value &lt; 0.01)</t>
   </si>
   <si>
     <t>Concept Match NOTA vs. Max Freq</t>
   </si>
   <si>
-    <t>H0:  Agent accuracy = 55%</t>
-  </si>
-  <si>
-    <t>H1: Agent accuracy &gt; 55%</t>
-  </si>
-  <si>
     <t>(0.01 &lt; p-value &lt; 0.02)</t>
   </si>
   <si>
@@ -106,6 +88,33 @@
   </si>
   <si>
     <t>Multiple Choice Questions</t>
+  </si>
+  <si>
+    <t>H0:  Agent accuracy = 48.0%</t>
+  </si>
+  <si>
+    <t>H1: Agent accuracy &gt; 48.0%</t>
+  </si>
+  <si>
+    <t>H0:  Agent accuracy = 67.3%</t>
+  </si>
+  <si>
+    <t>H1: Agent accuracy &gt; 67.3%</t>
+  </si>
+  <si>
+    <t>Conclusion: Accept H0.</t>
+  </si>
+  <si>
+    <t>H0:  Agent accuracy = 56.5%</t>
+  </si>
+  <si>
+    <t>H1: Agent accuracy &gt; 56.5%</t>
+  </si>
+  <si>
+    <t>H0:  Agent accuracy = 47%</t>
+  </si>
+  <si>
+    <t>H1: Agent accuracy &gt; 47%</t>
   </si>
 </sst>
 </file>
@@ -566,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H100"/>
+  <dimension ref="B2:I100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="K95" sqref="K95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -586,12 +595,12 @@
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:4">
@@ -599,7 +608,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.45400000000000001</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="8" spans="2:4">
@@ -608,7 +617,7 @@
       </c>
       <c r="D8">
         <f>D7*(1-D7)</f>
-        <v>0.24788400000000002</v>
+        <v>0.24959999999999999</v>
       </c>
     </row>
     <row r="9" spans="2:4">
@@ -616,7 +625,7 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>196</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -625,7 +634,7 @@
       </c>
       <c r="D10">
         <f>D9*D7</f>
-        <v>88.984000000000009</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="2:4">
@@ -634,7 +643,7 @@
       </c>
       <c r="D11">
         <f>D9*D8</f>
-        <v>48.585264000000002</v>
+        <v>37.44</v>
       </c>
     </row>
     <row r="12" spans="2:4">
@@ -643,7 +652,7 @@
       </c>
       <c r="D12">
         <f>SQRT(D11)</f>
-        <v>6.9703130489239866</v>
+        <v>6.1188234163113417</v>
       </c>
     </row>
     <row r="13" spans="2:4">
@@ -651,7 +660,7 @@
         <v>5</v>
       </c>
       <c r="D13">
-        <v>118</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="2:4">
@@ -660,7 +669,7 @@
       </c>
       <c r="D14">
         <f>(D13-D10)/D12</f>
-        <v>4.1627972511907796</v>
+        <v>4.7394732658394476</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -673,7 +682,7 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -683,12 +692,12 @@
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -696,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>0.60199999999999998</v>
+        <v>0.67300000000000004</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -705,7 +714,7 @@
       </c>
       <c r="D28">
         <f>D27*(1-D27)</f>
-        <v>0.239596</v>
+        <v>0.22007099999999999</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -713,7 +722,7 @@
         <v>17</v>
       </c>
       <c r="D29">
-        <v>196</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -722,7 +731,7 @@
       </c>
       <c r="D30">
         <f>D29*D27</f>
-        <v>117.99199999999999</v>
+        <v>100.95</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -731,7 +740,7 @@
       </c>
       <c r="D31">
         <f>D29*D28</f>
-        <v>46.960816000000001</v>
+        <v>33.010649999999998</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -740,7 +749,7 @@
       </c>
       <c r="D32">
         <f>SQRT(D31)</f>
-        <v>6.8527962176034389</v>
+        <v>5.7454895352789563</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -748,7 +757,7 @@
         <v>5</v>
       </c>
       <c r="D33">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -757,7 +766,7 @@
       </c>
       <c r="D34">
         <f>(D33-D30)/D32</f>
-        <v>0.43894490722970425</v>
+        <v>0.70490077044468247</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -845,7 +854,7 @@
         <v>5</v>
       </c>
       <c r="D53">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="2:4">
@@ -854,7 +863,7 @@
       </c>
       <c r="D54">
         <f>(D53-D50)/D52</f>
-        <v>2.3333333333333335</v>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="55" spans="2:4">
@@ -867,22 +876,22 @@
     </row>
     <row r="57" spans="2:4">
       <c r="B57" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="2:4">
       <c r="B62" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="2:8">
       <c r="B65" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="2:8">
@@ -890,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="D67">
-        <v>0.55000000000000004</v>
+        <v>0.56499999999999995</v>
       </c>
     </row>
     <row r="68" spans="2:8">
@@ -899,7 +908,7 @@
       </c>
       <c r="D68">
         <f>D67*(1-D67)</f>
-        <v>0.2475</v>
+        <v>0.24577499999999999</v>
       </c>
     </row>
     <row r="69" spans="2:8">
@@ -907,7 +916,7 @@
         <v>17</v>
       </c>
       <c r="D69">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="2:8">
@@ -916,7 +925,7 @@
       </c>
       <c r="D70">
         <f>D69*D67</f>
-        <v>92.95</v>
+        <v>91.529999999999987</v>
       </c>
     </row>
     <row r="71" spans="2:8">
@@ -925,7 +934,7 @@
       </c>
       <c r="D71">
         <f>D69*D68</f>
-        <v>41.827500000000001</v>
+        <v>39.815550000000002</v>
       </c>
     </row>
     <row r="72" spans="2:8">
@@ -934,7 +943,7 @@
       </c>
       <c r="D72">
         <f>SQRT(D71)</f>
-        <v>6.4674183411930297</v>
+        <v>6.3099564182330132</v>
       </c>
     </row>
     <row r="73" spans="2:8">
@@ -942,7 +951,7 @@
         <v>5</v>
       </c>
       <c r="D73">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H73">
         <f>9*1663</f>
@@ -955,7 +964,7 @@
       </c>
       <c r="D74">
         <f>(D73-D70)/D72</f>
-        <v>2.1724278929833734</v>
+        <v>2.2932012585995118</v>
       </c>
       <c r="H74">
         <v>6</v>
@@ -988,27 +997,27 @@
     </row>
     <row r="79" spans="2:8">
       <c r="B79" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="2:4">
       <c r="B84" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="85" spans="2:4">
       <c r="B85" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" spans="2:4">
       <c r="B87" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="2:4">
       <c r="B88" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="90" spans="2:4">
@@ -1033,7 +1042,7 @@
         <v>17</v>
       </c>
       <c r="D92">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="93" spans="2:4">
@@ -1042,7 +1051,7 @@
       </c>
       <c r="D93">
         <f>D92*D90</f>
-        <v>414.036</v>
+        <v>413.55899999999997</v>
       </c>
     </row>
     <row r="94" spans="2:4">
@@ -1051,7 +1060,7 @@
       </c>
       <c r="D94">
         <f>D92*D91</f>
-        <v>216.540828</v>
+        <v>216.291357</v>
       </c>
     </row>
     <row r="95" spans="2:4">
@@ -1060,7 +1069,7 @@
       </c>
       <c r="D95">
         <f>SQRT(D94)</f>
-        <v>14.715326296076482</v>
+        <v>14.706847282813539</v>
       </c>
     </row>
     <row r="96" spans="2:4">
@@ -1068,19 +1077,23 @@
         <v>5</v>
       </c>
       <c r="D96">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9">
       <c r="B97" t="s">
         <v>6</v>
       </c>
       <c r="D97">
         <f>(D96-D93)/D95</f>
-        <v>4.8904114358094537</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4">
+        <v>6.0135934166768985</v>
+      </c>
+      <c r="I97">
+        <f>D92*0.579</f>
+        <v>501.99299999999994</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9">
       <c r="B98" t="s">
         <v>7</v>
       </c>
@@ -1088,7 +1101,7 @@
         <v>2.3250000000000002</v>
       </c>
     </row>
-    <row r="100" spans="2:4">
+    <row r="100" spans="2:9">
       <c r="B100" t="s">
         <v>14</v>
       </c>

</xml_diff>